<commit_message>
staff management with API and windows service
</commit_message>
<xml_diff>
--- a/Mark1.xlsx
+++ b/Mark1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dotnetcore samples\Staff and student management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5EE7FF-C6F2-418B-BCEE-7BDE1AD6F35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42891693-5F43-441E-AF14-04567E48E8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1460D06E-7352-4D00-9D68-C7C6D28C89A9}"/>
+    <workbookView xWindow="5430" yWindow="330" windowWidth="15375" windowHeight="7875" xr2:uid="{1460D06E-7352-4D00-9D68-C7C6D28C89A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,11 +510,11 @@
         <v>45</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G6" si="0">SUM(C3:F3)</f>
+        <f>SUM(C3:F3)</f>
         <v>264</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H6" si="1">AVERAGE(C3:F3)</f>
+        <f>AVERAGE(C3:F3)</f>
         <v>66</v>
       </c>
     </row>
@@ -538,11 +538,11 @@
         <v>36</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
+        <f>SUM(C4:F4)</f>
         <v>220</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(C4:F4)</f>
         <v>55</v>
       </c>
     </row>
@@ -566,11 +566,11 @@
         <v>36</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f>SUM(C5:F5)</f>
         <v>244</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(C5:F5)</f>
         <v>61</v>
       </c>
     </row>
@@ -581,6 +581,9 @@
       <c r="B6" t="s">
         <v>12</v>
       </c>
+      <c r="C6">
+        <v>85</v>
+      </c>
       <c r="D6">
         <v>45</v>
       </c>
@@ -591,12 +594,12 @@
         <v>36</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>159</v>
+        <f>SUM(C6:F6)</f>
+        <v>244</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>53</v>
+        <f>AVERAGE(C6:F6)</f>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>